<commit_message>
EDIT Stückliste changed to farnell and rs
</commit_message>
<xml_diff>
--- a/hardware/Stückliste.xlsx
+++ b/hardware/Stückliste.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastian/Documents/Schule/Fachhochschule/Semester_5/Digitale Messtechnik/project/hardware/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{245047C5-33B6-5C46-9D29-149284C909B7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01D20832-B823-094C-9B4D-B461768EAA20}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6280" yWindow="5000" windowWidth="25440" windowHeight="14540" xr2:uid="{C767C699-CF08-BC4F-AEAA-E2396BB6BB90}"/>
+    <workbookView xWindow="2280" yWindow="3860" windowWidth="27480" windowHeight="15460" xr2:uid="{C767C699-CF08-BC4F-AEAA-E2396BB6BB90}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
   <si>
     <t>Bauteil</t>
   </si>
@@ -51,21 +51,12 @@
     <t>ADA4891</t>
   </si>
   <si>
-    <t>ADA4891-2ARZ-R7CT-ND</t>
-  </si>
-  <si>
     <t>Gurtabschnitt (CT)</t>
   </si>
   <si>
     <t>8-SOIC</t>
   </si>
   <si>
-    <t>digikey.at</t>
-  </si>
-  <si>
-    <t>https://www.digikey.at/product-detail/de/analog-devices-inc/ADA4891-2ARZ-R7/ADA4891-2ARZ-R7CT-ND/3828899</t>
-  </si>
-  <si>
     <t>Potentiometer</t>
   </si>
   <si>
@@ -81,27 +72,15 @@
     <t>SOIC to DIP Adapter</t>
   </si>
   <si>
-    <t>https://www.digikey.at/product-detail/de/sparkfun-electronics/BOB-13655/1568-1123-ND/5528943</t>
-  </si>
-  <si>
-    <t>1568-1123-ND</t>
-  </si>
-  <si>
     <t>Widerstand</t>
   </si>
   <si>
     <t>Kondensator</t>
   </si>
   <si>
-    <t>https://www.digikey.at/product-detail/de/texas-instruments/LM2776DBVR/296-43957-1-ND/5973203</t>
-  </si>
-  <si>
     <t>LM2776DBVR</t>
   </si>
   <si>
-    <t>296-43957-1-ND</t>
-  </si>
-  <si>
     <t>SOT-23-6</t>
   </si>
   <si>
@@ -120,24 +99,6 @@
     <t>Summe</t>
   </si>
   <si>
-    <t>https://www.digikey.at/product-detail/de/tdk-corporation/FG28C0G1H4R7CNT06/445-173502-1-ND/5812107</t>
-  </si>
-  <si>
-    <t>FHTW od. digikey.at</t>
-  </si>
-  <si>
-    <t>Digikey Teilenummer</t>
-  </si>
-  <si>
-    <t>445-173502-1-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.at/product-detail/de/kemet/C330C105K5R5TA7301/399-9886-1-ND/3726180</t>
-  </si>
-  <si>
-    <t>399-9886-1-ND</t>
-  </si>
-  <si>
     <t>OPV</t>
   </si>
   <si>
@@ -147,50 +108,57 @@
     <t>Spannungsinverter</t>
   </si>
   <si>
-    <t>445-173260-1-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.at/product-detail/de/tdk-corporation/FG18X7R1A225KRT06/445-173260-1-ND/5811865</t>
-  </si>
-  <si>
-    <t>https://www.digikey.at/product-detail/de/stackpole-electronics-inc/RNF14FTD10K0/RNF14FTD10K0CT-ND/1975090</t>
-  </si>
-  <si>
-    <t>RNF14FTD10K0CT-ND</t>
-  </si>
-  <si>
     <t>Preis gesammt</t>
   </si>
   <si>
-    <t>https://www.digikey.at/product-detail/de/tt-electronics-bi/P160KN2-0QA25B10K/987-1715-ND/5957459</t>
-  </si>
-  <si>
-    <t>987-1715-ND</t>
-  </si>
-  <si>
-    <t>Tablett</t>
+    <t>FHTW</t>
+  </si>
+  <si>
+    <t>rs-online.com</t>
+  </si>
+  <si>
+    <t>https://at.rs-online.com/web/p/operationsverstarker/7591534/?relevancy-data=636F3D3126696E3D4931384E53656172636847656E65726963266C753D6465266D6D3D6D61746368616C6C7061727469616C26706D3D5E5B5C707B4C7D5C707B4E647D2D2C2F255C2E5D2B2426706F3D31333326736E3D592673723D2673743D4B4559574F52445F53494E474C455F414C5048415F4E554D455249432673633D592677633D4E4F4E45267573743D414441343839312D3241525A267374613D414441343839312D3241525A26&amp;searchHistory=%7B%22enabled%22%3Atrue%7D</t>
+  </si>
+  <si>
+    <t>https://at.farnell.com/texas-instruments/lm2776dbvr/dc-dc-ladungspumpe-invertierend/dp/2817376?st=LM2776DBVR</t>
+  </si>
+  <si>
+    <t>farnell.com</t>
+  </si>
+  <si>
+    <t>Farnell Bestellnummer</t>
+  </si>
+  <si>
+    <t>RS-Online Bestellnummer</t>
+  </si>
+  <si>
+    <t>759-1534</t>
+  </si>
+  <si>
+    <t>https://at.farnell.com/aries/lcqt-soic8-8/ic-adapter-8-soic-dip-2-54mm/dp/2476033?st=SOIC%20Adapter</t>
+  </si>
+  <si>
+    <t>Abschluss</t>
+  </si>
+  <si>
+    <t>✔️</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$€-2]\ #,##0.00;[Red]\-[$€-2]\ #,##0.00"/>
+    <numFmt numFmtId="169" formatCode="[$€-2]\ #,##0.000;[Red]\-[$€-2]\ #,##0.000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -231,12 +199,12 @@
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -551,290 +519,253 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{998F31DA-849B-4441-A2B2-EEC25BFB9502}">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.6640625" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="24.6640625" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="2">
+        <v>1.94</v>
+      </c>
+      <c r="K2" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3">
+        <v>2476033</v>
+      </c>
+      <c r="J3" s="2">
+        <v>4.21</v>
+      </c>
+      <c r="K3" t="s">
+        <v>32</v>
+      </c>
+      <c r="L3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4">
+        <v>2817376</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="6">
+        <v>0.85299999999999998</v>
+      </c>
+      <c r="K4" t="s">
+        <v>32</v>
+      </c>
+      <c r="L4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" s="2"/>
+      <c r="K5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" t="s">
         <v>15</v>
       </c>
-      <c r="F1" t="s">
+      <c r="C6">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2">
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" s="2"/>
+      <c r="K6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" s="4"/>
+      <c r="K7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="J8" s="4"/>
+      <c r="K8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="3">
-        <v>1.86</v>
-      </c>
-      <c r="I2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="3">
-        <v>2.59</v>
-      </c>
-      <c r="I3" t="s">
-        <v>11</v>
-      </c>
-      <c r="J3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
+      <c r="J9" s="4"/>
+      <c r="K9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J10" s="3"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B11" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H4" s="3">
-        <v>0.92</v>
-      </c>
-      <c r="I4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="F5" s="1"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="3"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" t="s">
-        <v>47</v>
-      </c>
-      <c r="H6" s="3">
-        <v>1.38</v>
-      </c>
-      <c r="I6" t="s">
-        <v>32</v>
-      </c>
-      <c r="J6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7">
-        <v>3</v>
-      </c>
-      <c r="C7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" t="s">
-        <v>43</v>
-      </c>
-      <c r="F7" t="s">
-        <v>9</v>
-      </c>
-      <c r="H7" s="3">
-        <v>0.27</v>
-      </c>
-      <c r="I7" t="s">
-        <v>32</v>
-      </c>
-      <c r="J7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8">
-        <v>2</v>
-      </c>
-      <c r="C8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F8" t="s">
-        <v>9</v>
-      </c>
-      <c r="H8" s="5">
-        <v>0.42</v>
-      </c>
-      <c r="I8" t="s">
-        <v>32</v>
-      </c>
-      <c r="J8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9">
-        <v>2</v>
-      </c>
-      <c r="C9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F9" t="s">
-        <v>9</v>
-      </c>
-      <c r="H9" s="5">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="I9" t="s">
-        <v>32</v>
-      </c>
-      <c r="J9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" t="s">
-        <v>36</v>
-      </c>
-      <c r="F10" t="s">
-        <v>9</v>
-      </c>
-      <c r="H10" s="5">
-        <v>0.48</v>
-      </c>
-      <c r="I10" t="s">
-        <v>32</v>
-      </c>
-      <c r="J10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="H11" s="4"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="7">
-        <f>SUM(H2:H10)</f>
-        <v>8.48</v>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="7">
+        <f>SUM(J2:J9)</f>
+        <v>7.0030000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
EDIT Stückliste Link update
</commit_message>
<xml_diff>
--- a/hardware/Stückliste.xlsx
+++ b/hardware/Stückliste.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastian/Documents/Schule/Fachhochschule/Semester_5/Digitale Messtechnik/project/hardware/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01D20832-B823-094C-9B4D-B461768EAA20}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24B54FF7-57AB-3D4E-913D-ABE76F17E9F5}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="3860" windowWidth="27480" windowHeight="15460" xr2:uid="{C767C699-CF08-BC4F-AEAA-E2396BB6BB90}"/>
+    <workbookView xWindow="5240" yWindow="3980" windowWidth="27480" windowHeight="15460" xr2:uid="{C767C699-CF08-BC4F-AEAA-E2396BB6BB90}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -150,9 +150,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$€-2]\ #,##0.00;[Red]\-[$€-2]\ #,##0.00"/>
-    <numFmt numFmtId="169" formatCode="[$€-2]\ #,##0.000;[Red]\-[$€-2]\ #,##0.000"/>
+    <numFmt numFmtId="165" formatCode="[$€-2]\ #,##0.000;[Red]\-[$€-2]\ #,##0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -175,6 +175,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -184,7 +192,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -192,21 +200,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -519,10 +540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{998F31DA-849B-4441-A2B2-EEC25BFB9502}">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -538,40 +559,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="4" t="s">
         <v>5</v>
       </c>
     </row>
@@ -600,7 +621,7 @@
       <c r="K2" t="s">
         <v>29</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="6" t="s">
         <v>30</v>
       </c>
     </row>
@@ -623,7 +644,7 @@
       <c r="K3" t="s">
         <v>32</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" s="6" t="s">
         <v>36</v>
       </c>
     </row>
@@ -646,13 +667,13 @@
       <c r="I4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J4" s="6">
+      <c r="J4" s="5">
         <v>0.85299999999999998</v>
       </c>
       <c r="K4" t="s">
         <v>32</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" s="6" t="s">
         <v>31</v>
       </c>
     </row>
@@ -708,7 +729,7 @@
       <c r="D7" t="s">
         <v>20</v>
       </c>
-      <c r="J7" s="4"/>
+      <c r="J7" s="3"/>
       <c r="K7" t="s">
         <v>28</v>
       </c>
@@ -726,7 +747,7 @@
       <c r="D8" t="s">
         <v>21</v>
       </c>
-      <c r="J8" s="4"/>
+      <c r="J8" s="3"/>
       <c r="K8" t="s">
         <v>28</v>
       </c>
@@ -744,31 +765,35 @@
       <c r="D9" t="s">
         <v>22</v>
       </c>
-      <c r="J9" s="4"/>
+      <c r="J9" s="3"/>
       <c r="K9" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="J10" s="3"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B11" s="5" t="s">
+      <c r="A10" s="7"/>
+      <c r="B10" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="7">
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="9">
         <f>SUM(J2:J9)</f>
         <v>7.0030000000000001</v>
       </c>
+      <c r="K10" s="7"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="L2" r:id="rId1" display="https://at.rs-online.com/web/p/operationsverstarker/7591534/?relevancy-data=636F3D3126696E3D4931384E53656172636847656E65726963266C753D6465266D6D3D6D61746368616C6C7061727469616C26706D3D5E5B5C707B4C7D5C707B4E647D2D2C2F255C2E5D2B2426706F3D31333326736E3D592673723D2673743D4B4559574F52445F53494E474C455F414C5048415F4E554D455249432673633D592677633D4E4F4E45267573743D414441343839312D3241525A267374613D414441343839312D3241525A26&amp;searchHistory=%7B%22enabled%22%3Atrue%7D" xr:uid="{118AB77E-E600-5746-9F3C-51AB9D93BE9D}"/>
+    <hyperlink ref="L3" r:id="rId2" xr:uid="{9FD840A4-1ACA-B14F-952B-BBF39605F0F6}"/>
+    <hyperlink ref="L4" r:id="rId3" xr:uid="{AD0F6464-39D1-B849-B0BB-27C2218122D5}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
EDIT Stückliste new adapter / removed unused files
</commit_message>
<xml_diff>
--- a/hardware/Stückliste.xlsx
+++ b/hardware/Stückliste.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastian/Documents/Schule/Fachhochschule/Semester_5/Digitale Messtechnik/project/hardware/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24B54FF7-57AB-3D4E-913D-ABE76F17E9F5}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0DC22D3-AC04-9D4E-907C-117C6D46A367}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5240" yWindow="3980" windowWidth="27480" windowHeight="15460" xr2:uid="{C767C699-CF08-BC4F-AEAA-E2396BB6BB90}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
   <si>
     <t>Bauteil</t>
   </si>
@@ -117,9 +117,6 @@
     <t>rs-online.com</t>
   </si>
   <si>
-    <t>https://at.rs-online.com/web/p/operationsverstarker/7591534/?relevancy-data=636F3D3126696E3D4931384E53656172636847656E65726963266C753D6465266D6D3D6D61746368616C6C7061727469616C26706D3D5E5B5C707B4C7D5C707B4E647D2D2C2F255C2E5D2B2426706F3D31333326736E3D592673723D2673743D4B4559574F52445F53494E474C455F414C5048415F4E554D455249432673633D592677633D4E4F4E45267573743D414441343839312D3241525A267374613D414441343839312D3241525A26&amp;searchHistory=%7B%22enabled%22%3Atrue%7D</t>
-  </si>
-  <si>
     <t>https://at.farnell.com/texas-instruments/lm2776dbvr/dc-dc-ladungspumpe-invertierend/dp/2817376?st=LM2776DBVR</t>
   </si>
   <si>
@@ -142,14 +139,22 @@
   </si>
   <si>
     <t>✔️</t>
+  </si>
+  <si>
+    <t>SOT23 to DIP Adapter</t>
+  </si>
+  <si>
+    <t>https://at.farnell.com/capital-advanced/33206/steckverbinder-smd-ic-adapter/dp/1654365?ost=1654365</t>
+  </si>
+  <si>
+    <t>https://at.rs-online.com/web/p/operationsverstarker/7591534/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="[$€-2]\ #,##0.00;[Red]\-[$€-2]\ #,##0.00"/>
+  <numFmts count="1">
     <numFmt numFmtId="165" formatCode="[$€-2]\ #,##0.000;[Red]\-[$€-2]\ #,##0.000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
@@ -214,17 +219,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -540,59 +544,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{998F31DA-849B-4441-A2B2-EEC25BFB9502}">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="24.6640625" customWidth="1"/>
+    <col min="5" max="5" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="101.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F1" s="4" t="s">
+      <c r="E1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="F1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -607,7 +615,7 @@
         <v>24</v>
       </c>
       <c r="E2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H2" t="s">
         <v>8</v>
@@ -615,14 +623,14 @@
       <c r="I2" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="2">
+      <c r="J2" s="3">
         <v>1.94</v>
       </c>
       <c r="K2" t="s">
         <v>29</v>
       </c>
-      <c r="L2" s="6" t="s">
-        <v>30</v>
+      <c r="L2" s="4" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -638,14 +646,14 @@
       <c r="F3">
         <v>2476033</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3" s="3">
         <v>4.21</v>
       </c>
       <c r="K3" t="s">
-        <v>32</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>36</v>
+        <v>31</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -667,67 +675,74 @@
       <c r="I4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J4" s="5">
+      <c r="J4" s="3">
         <v>0.85299999999999998</v>
       </c>
       <c r="K4" t="s">
-        <v>32</v>
-      </c>
-      <c r="L4" s="6" t="s">
         <v>31</v>
       </c>
+      <c r="L4" s="4" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
         <v>38</v>
       </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
       <c r="C5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" t="s">
-        <v>13</v>
-      </c>
-      <c r="J5" s="2"/>
+        <v>25</v>
+      </c>
+      <c r="F5">
+        <v>1654365</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="3">
+        <v>1.51</v>
+      </c>
       <c r="K5" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J6" s="2"/>
+        <v>11</v>
+      </c>
+      <c r="G6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" s="3"/>
       <c r="K6" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J7" s="3"/>
       <c r="K7" t="s">
@@ -736,7 +751,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B8" t="s">
         <v>16</v>
@@ -745,52 +760,70 @@
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>21</v>
-      </c>
-      <c r="J8" s="3"/>
+        <v>20</v>
+      </c>
+      <c r="J8" s="8"/>
       <c r="K8" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B9" t="s">
         <v>16</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>22</v>
-      </c>
-      <c r="J9" s="3"/>
+        <v>21</v>
+      </c>
+      <c r="J9" s="8"/>
       <c r="K9" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="7"/>
-      <c r="B10" s="8" t="s">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>22</v>
+      </c>
+      <c r="J10" s="8"/>
+      <c r="K10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" s="5"/>
+      <c r="B11" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="9">
-        <f>SUM(J2:J9)</f>
-        <v>7.0030000000000001</v>
-      </c>
-      <c r="K10" s="7"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="7">
+        <f>SUM(J2:J10)</f>
+        <v>8.5129999999999999</v>
+      </c>
+      <c r="K11" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1" display="https://at.rs-online.com/web/p/operationsverstarker/7591534/?relevancy-data=636F3D3126696E3D4931384E53656172636847656E65726963266C753D6465266D6D3D6D61746368616C6C7061727469616C26706D3D5E5B5C707B4C7D5C707B4E647D2D2C2F255C2E5D2B2426706F3D31333326736E3D592673723D2673743D4B4559574F52445F53494E474C455F414C5048415F4E554D455249432673633D592677633D4E4F4E45267573743D414441343839312D3241525A267374613D414441343839312D3241525A26&amp;searchHistory=%7B%22enabled%22%3Atrue%7D" xr:uid="{118AB77E-E600-5746-9F3C-51AB9D93BE9D}"/>
+    <hyperlink ref="L2" r:id="rId1" xr:uid="{118AB77E-E600-5746-9F3C-51AB9D93BE9D}"/>
     <hyperlink ref="L3" r:id="rId2" xr:uid="{9FD840A4-1ACA-B14F-952B-BBF39605F0F6}"/>
     <hyperlink ref="L4" r:id="rId3" xr:uid="{AD0F6464-39D1-B849-B0BB-27C2218122D5}"/>
   </hyperlinks>

</xml_diff>

<commit_message>
EDIT: Presentation ADD: IMAGES
</commit_message>
<xml_diff>
--- a/hardware/Stückliste.xlsx
+++ b/hardware/Stückliste.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastian/Documents/Schule/Fachhochschule/Semester_5/Digitale Messtechnik/project/hardware/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0DC22D3-AC04-9D4E-907C-117C6D46A367}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C164B41-BE21-B049-8C3F-1BE9C96C218F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5240" yWindow="3980" windowWidth="27480" windowHeight="15460" xr2:uid="{C767C699-CF08-BC4F-AEAA-E2396BB6BB90}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="41">
   <si>
     <t>Bauteil</t>
   </si>
@@ -155,7 +155,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$€-2]\ #,##0.000;[Red]\-[$€-2]\ #,##0.000"/>
+    <numFmt numFmtId="164" formatCode="[$€-2]\ #,##0.000;[Red]\-[$€-2]\ #,##0.000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -223,12 +223,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -547,7 +547,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -605,6 +605,9 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
@@ -634,6 +637,9 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
       <c r="B3" t="s">
         <v>14</v>
       </c>
@@ -657,6 +663,9 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>37</v>
+      </c>
       <c r="B4" t="s">
         <v>17</v>
       </c>
@@ -686,6 +695,9 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
       <c r="B5" t="s">
         <v>38</v>
       </c>

</xml_diff>